<commit_message>
15-01-26; Implementando la app de Escritorio con Python
</commit_message>
<xml_diff>
--- a/Archivos varios/Excel para SCORE2/SCORE2_PruebaFinal.xlsx
+++ b/Archivos varios/Excel para SCORE2/SCORE2_PruebaFinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Hernán\Desktop\Administracion HernanMayol\Python_ISSUNNE\Archivos varios\Excel para SCORE2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04480C02-0BA9-49BC-BD24-6F0E09EA814B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B504D1-506C-4F21-AF45-BB6B361C1BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="11070" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pacientes" sheetId="1" r:id="rId1"/>
@@ -3869,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4177,8 +4177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,7 +4679,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4822,7 +4822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF5B978-4E49-4A1C-B860-2F48D05AFACD}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -5139,7 +5139,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>